<commit_message>
Coding till Feature Selection Complete
</commit_message>
<xml_diff>
--- a/Codes/FIF Evaluation.xlsx
+++ b/Codes/FIF Evaluation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashis\Desktop\RToS\Codes\MicroService Architecture V 2.0\LDA_Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashis\Desktop\RToS\Codes\MicroService Architecture V 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{027F1F19-DBAA-446E-9D3C-9259E956DBE5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{838CF054-B881-40E8-8581-9E83A81F7E9F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30" yWindow="30" windowWidth="20445" windowHeight="10890" xr2:uid="{CEB951F8-7FF4-4FD7-AAA5-5F9776E32682}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="56">
   <si>
     <t>User Story</t>
   </si>
@@ -48,9 +48,6 @@
     <t>As a supply chain analyst, I want to analyze the sales data for newly opened supermarket store on a fortnightly basis so that I can identify inventory demand patterns for the next quarter.</t>
   </si>
   <si>
-    <t>As a supermarket store manager , I want to find the relationship between the visibility of products present in store and other characteristics such as item and type of store so that I can organize the products in the store.</t>
-  </si>
-  <si>
     <t>As a store manager, I want to group all the products that were bought together by the customers in the last quarter so that I can find which products are sold together.</t>
   </si>
   <si>
@@ -58,9 +55,6 @@
   </si>
   <si>
     <t>As a movie critic, I want to segregate the movies based on their genre and actors present in the movie so that I can focus on a similar type of a movie.</t>
-  </si>
-  <si>
-    <t>As a Sports Analyst, I want to gather the information about a player and a team that received the maximum number of awards so that I am able to analyze the specific team and players played during the season.</t>
   </si>
   <si>
     <t>As a company human resource manager, I want to gather information about employees under a specific manager so that information can be useful for new organization restructuring.</t>
@@ -93,6 +87,118 @@
   </si>
   <si>
     <t>As a supermarket sales executive, I want to guide the employees in order to arrange the products based on weight of item and fat contain so that sales of specific product can be increased.</t>
+  </si>
+  <si>
+    <t>super_market or Walmart</t>
+  </si>
+  <si>
+    <t>sakila</t>
+  </si>
+  <si>
+    <t>As a Sports Analyst, I want to gather the information about a basketball player and a team that received the maximum number of awards so that I am able to analyze the specific team and players played during the season.</t>
+  </si>
+  <si>
+    <t>basketball_men or basketball_women</t>
+  </si>
+  <si>
+    <t>employee</t>
+  </si>
+  <si>
+    <t>Relevant Tables</t>
+  </si>
+  <si>
+    <t>item_outlet_fact, outlet_information, item_information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Item_Outlet_sales, Item_Identifier, Item_MRP, Item_Type,
+Outlet_Identifier, Outlet_Size, Outlet_Type, Outlet_Location_Type </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Item_Outlet_sales, Item_Identifier,
+Outlet_Identifier, Outlet_Size, Outlet_Type, Outlet_Location_Type </t>
+  </si>
+  <si>
+    <t>outlet_information</t>
+  </si>
+  <si>
+    <t>outlet_information, item_information, item_outlet_fact</t>
+  </si>
+  <si>
+    <t>Outlet_Identifier, Item_Identifier, Item_Outlet_sale, Item_Weight, Item_Fat_Content, Item_Type</t>
+  </si>
+  <si>
+    <t>Item_Identifier, Item_Outlet_sale, Item_Weight, Item_Fat_Content, Item_Type</t>
+  </si>
+  <si>
+    <t>As a supermarket store manager , I want to find the relationship between the visibility of products present in store and other characteristics such as type of store, type of product so that I can organize the products in the store.</t>
+  </si>
+  <si>
+    <t>Item_Identifier, Item_Visibility, Item_Type, Outlet_Identifier, Outlet_Type,   Outlet_Size, Outlet_Location_Type</t>
+  </si>
+  <si>
+    <t>Item_Identifier, Item_Visibility, Item_Type,  Outlet_Type</t>
+  </si>
+  <si>
+    <t>outlet_information, item_information</t>
+  </si>
+  <si>
+    <t>Item_Identifier, Item_Type, Item_Visibility, Item_MRP, Item_Outlet_Sales</t>
+  </si>
+  <si>
+    <t>Item_Identifier, Item_Type, Item_Visibility, Item_MRP, Item_Outlet_Sales, Outlet_Identifier</t>
+  </si>
+  <si>
+    <t>Outlet_Identifier,
+Outlet_establishment_year, Outlet_Size, Outlet_Type, Outlet_Location_Type</t>
+  </si>
+  <si>
+    <t>Outlet_Identifier,
+Outlet_Size, Outlet_Type</t>
+  </si>
+  <si>
+    <t>actor, category, film, film_actor, film_category,  film_text, language</t>
+  </si>
+  <si>
+    <t>actor_id, actor|first_name, actor|last_name, category_id, name, film_id , title, description, release_year, language_id, rating, special features, language|name</t>
+  </si>
+  <si>
+    <t>film, inventory, payment, rental</t>
+  </si>
+  <si>
+    <t>film_id, title, release_year, rental_duration, rental_rate, length, replacement_cost, inventory_id, store_id, payment_id, rental_id, amount, payment_date, rental_date, return_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">film_id, title,  rental_duration, rental_rate, payment_id, rental_id, amount, </t>
+  </si>
+  <si>
+    <t>actor_id, actor|first_name, actor|last_name, category_id, name, film_id , title, language|name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coach|id, coachID, coach|award, playerID, player|award, player|year, coach|year, player|lgID, coach|lgID, player|pos, tmID, won, lost, post_wins, post_losses, last_name, first_name, season_id, conference, league_id, games_played, minutes, points, o_rebounds, d_rebounds, rebounds, assists, steals, blocks, turnover, personal_fouls, fg_attempted, fg_made, ft_attempted, ft_made, three_attempted, three_made, useFirst, firstName, middleName, lastName, </t>
+  </si>
+  <si>
+    <t>coach|id, coachID, coach|award, playerID, player|award, player|pos, tmID, last_name, first_name, season_id, conference, league_id</t>
+  </si>
+  <si>
+    <t>award_coaches, award_players, coaches, player_allstar, players, players_team, teams</t>
+  </si>
+  <si>
+    <t>departments, dept_emp, dept_manager,salaries, titles</t>
+  </si>
+  <si>
+    <t>dept_no, dept_name, dept_emp|emp_no, dept_manager|emp_no</t>
+  </si>
+  <si>
+    <t>dept_no, dept_name, dept_emp|emp_no, dept_manager|emp_no,  salary, from_date, to_date, title</t>
+  </si>
+  <si>
+    <t>dept_emp|dept_no, dept_manager|dept_no, dept_name, dept_emp|emp_no, dept_manager|emp_no,  hire_date,  salary|emp_no, salary, from_date, to_date, title</t>
+  </si>
+  <si>
+    <t>dept_no,  hire_date,  salary|emp_no, salary, title</t>
+  </si>
+  <si>
+    <t>departments, dept_emp, dept_manager, salaries, titles</t>
   </si>
 </sst>
 </file>
@@ -152,26 +258,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -487,277 +604,374 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53494CB1-07B4-40D1-A530-0E781A70A52C}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.42578125" customWidth="1"/>
-    <col min="2" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="6" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="1" max="1" width="45.42578125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="35.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" style="8" customWidth="1"/>
+    <col min="7" max="8" width="18.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19" style="8" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="6" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-    </row>
-    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+    </row>
+    <row r="2" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="2" t="s">
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="C7" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="C8" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="B9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="300" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="B11" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>15</v>
+      <c r="B12" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Finalised Version of FIF
</commit_message>
<xml_diff>
--- a/Codes/FIF Evaluation.xlsx
+++ b/Codes/FIF Evaluation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashis\Desktop\RToS\Codes\MicroService Architecture V 3.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E56AA35-F813-4267-822E-F9F63278D5CE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BF5AAE-83CF-40B4-B5F6-3CA4500513A6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30" yWindow="30" windowWidth="20445" windowHeight="10890" xr2:uid="{CEB951F8-7FF4-4FD7-AAA5-5F9776E32682}"/>
   </bookViews>
@@ -1286,7 +1286,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1312,6 +1312,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1319,13 +1336,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
@@ -1337,24 +1347,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1674,10 +1671,10 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1698,27 +1695,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="10" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
     </row>
     <row r="2" spans="1:12" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
+      <c r="A2" s="16"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1775,11 +1772,11 @@
       <c r="G3" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="I3" s="16"/>
-      <c r="J3" s="17"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="21"/>
       <c r="K3" s="7" t="s">
         <v>13</v>
       </c>
@@ -1809,11 +1806,11 @@
       <c r="G4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="20" t="s">
+      <c r="H4" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="I4" s="21"/>
-      <c r="J4" s="22"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="15"/>
       <c r="K4" s="7" t="s">
         <v>15</v>
       </c>
@@ -1843,11 +1840,11 @@
       <c r="G5" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="I5" s="21"/>
-      <c r="J5" s="22"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="15"/>
       <c r="K5" s="7" t="s">
         <v>15</v>
       </c>
@@ -1877,11 +1874,11 @@
       <c r="G6" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="H6" s="20" t="s">
+      <c r="H6" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="I6" s="21"/>
-      <c r="J6" s="22"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="15"/>
       <c r="K6" s="7" t="s">
         <v>14</v>
       </c>
@@ -1911,11 +1908,11 @@
       <c r="G7" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="H7" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="21"/>
-      <c r="J7" s="22"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="15"/>
       <c r="K7" s="7" t="s">
         <v>15</v>
       </c>
@@ -1945,11 +1942,11 @@
       <c r="G8" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="H8" s="20" t="s">
+      <c r="H8" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="I8" s="21"/>
-      <c r="J8" s="22"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="15"/>
       <c r="K8" s="7" t="s">
         <v>13</v>
       </c>
@@ -1979,11 +1976,11 @@
       <c r="G9" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="H9" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="I9" s="21"/>
-      <c r="J9" s="22"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="15"/>
       <c r="K9" s="7" t="s">
         <v>14</v>
       </c>
@@ -1992,7 +1989,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="300" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="8" t="s">
@@ -2013,11 +2010,11 @@
       <c r="G10" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="H10" s="20" t="s">
+      <c r="H10" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="I10" s="21"/>
-      <c r="J10" s="22"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="15"/>
       <c r="K10" s="7" t="s">
         <v>13</v>
       </c>
@@ -2047,11 +2044,11 @@
       <c r="G11" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="20" t="s">
+      <c r="H11" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="I11" s="21"/>
-      <c r="J11" s="22"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="15"/>
       <c r="K11" s="7" t="s">
         <v>15</v>
       </c>
@@ -2081,11 +2078,11 @@
       <c r="G12" s="7" t="s">
         <v>372</v>
       </c>
-      <c r="H12" s="20" t="s">
+      <c r="H12" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="I12" s="21"/>
-      <c r="J12" s="22"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="15"/>
       <c r="K12" s="7" t="s">
         <v>13</v>
       </c>
@@ -2095,6 +2092,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:L1"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="H4:J4"/>
     <mergeCell ref="H10:J10"/>
     <mergeCell ref="H11:J11"/>
     <mergeCell ref="H12:J12"/>
@@ -2103,11 +2105,6 @@
     <mergeCell ref="H7:J7"/>
     <mergeCell ref="H8:J8"/>
     <mergeCell ref="H9:J9"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="G1:L1"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="H4:J4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H3:J3" location="'User Story 1'!A1" display="user_ story_1" xr:uid="{E813C819-D1F7-4AC2-B2EA-001830550F7B}"/>
@@ -2130,9 +2127,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95CBB242-3A77-4F59-BA25-C7DA4891FB09}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -2166,25 +2161,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="11" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="10" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2310,20 +2305,20 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="10" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2504,25 +2499,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="11" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="10" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2631,20 +2626,20 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="10" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2803,25 +2798,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="12" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="10" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2919,20 +2914,20 @@
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="10" t="s">
         <v>90</v>
       </c>
     </row>
@@ -3079,96 +3074,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="12" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
     </row>
     <row r="3" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="10" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="9" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="9" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="9" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="9" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="9" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="9" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3178,20 +3173,20 @@
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
     </row>
     <row r="13" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="10" t="s">
         <v>90</v>
       </c>
     </row>
@@ -3201,79 +3196,79 @@
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="9" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="9" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="9" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="9" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="9" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="9" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="9" t="s">
         <v>82</v>
       </c>
     </row>
@@ -3305,140 +3300,140 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="12" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
     </row>
     <row r="3" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="10" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="9" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="9" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="9" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="9" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="9" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="9" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="9" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="9" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="9" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="9" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3448,20 +3443,20 @@
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
     </row>
     <row r="17" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="10" t="s">
         <v>90</v>
       </c>
     </row>
@@ -3471,134 +3466,134 @@
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="9" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="9" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="9" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="9" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="9" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="9" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="9" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="9" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="9" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="9" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="9" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="9" t="s">
         <v>82</v>
       </c>
     </row>
@@ -3630,25 +3625,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="12" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
     </row>
     <row r="3" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="10" t="s">
         <v>88</v>
       </c>
     </row>
@@ -3751,20 +3746,20 @@
       <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
     </row>
     <row r="15" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="10" t="s">
         <v>90</v>
       </c>
     </row>
@@ -4307,25 +4302,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="12" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
     </row>
     <row r="3" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="10" t="s">
         <v>88</v>
       </c>
     </row>
@@ -4395,20 +4390,20 @@
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
     </row>
     <row r="12" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="10" t="s">
         <v>90</v>
       </c>
     </row>
@@ -4728,7 +4723,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5AF8676-EB7F-401E-9709-763E862C14E7}">
-  <dimension ref="A1:C168"/>
+  <dimension ref="A1:H168"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4737,37 +4732,44 @@
     <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="89.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-    </row>
-    <row r="3" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+    </row>
+    <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="10" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>225</v>
       </c>
@@ -4777,8 +4779,11 @@
       <c r="C5" s="2" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>228</v>
       </c>
@@ -4788,8 +4793,11 @@
       <c r="C6" s="2" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>139</v>
       </c>
@@ -4799,8 +4807,11 @@
       <c r="C7" s="2" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>231</v>
       </c>
@@ -4810,8 +4821,11 @@
       <c r="C8" s="2" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>233</v>
       </c>
@@ -4821,8 +4835,11 @@
       <c r="C9" s="2" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>235</v>
       </c>
@@ -4832,8 +4849,10 @@
       <c r="C10" s="2" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F10" s="3"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>236</v>
       </c>
@@ -4843,8 +4862,10 @@
       <c r="C11" s="2" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F11" s="3"/>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>237</v>
       </c>
@@ -4854,8 +4875,10 @@
       <c r="C12" s="2" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F12" s="3"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>134</v>
       </c>
@@ -4865,8 +4888,10 @@
       <c r="C13" s="2" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F13" s="3"/>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>136</v>
       </c>
@@ -4876,8 +4901,10 @@
       <c r="C14" s="2" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F14" s="3"/>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>238</v>
       </c>
@@ -4887,36 +4914,38 @@
       <c r="C15" s="2" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F15" s="3"/>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
+    <row r="17" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-    </row>
-    <row r="18" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+    </row>
+    <row r="18" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="10" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>239</v>
       </c>
@@ -4926,8 +4955,10 @@
       <c r="C20" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F20" s="3"/>
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>242</v>
       </c>
@@ -4937,8 +4968,10 @@
       <c r="C21" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F21" s="3"/>
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>243</v>
       </c>
@@ -4948,8 +4981,10 @@
       <c r="C22" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F22" s="3"/>
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>244</v>
       </c>
@@ -4959,8 +4994,10 @@
       <c r="C23" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F23" s="3"/>
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>245</v>
       </c>
@@ -4970,8 +5007,10 @@
       <c r="C24" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F24" s="3"/>
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>244</v>
       </c>
@@ -4981,8 +5020,10 @@
       <c r="C25" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F25" s="3"/>
+      <c r="H25" s="3"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>247</v>
       </c>
@@ -4992,8 +5033,10 @@
       <c r="C26" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F26" s="3"/>
+      <c r="H26" s="3"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>248</v>
       </c>
@@ -5003,8 +5046,10 @@
       <c r="C27" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F27" s="3"/>
+      <c r="H27" s="3"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>249</v>
       </c>
@@ -5014,8 +5059,10 @@
       <c r="C28" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F28" s="3"/>
+      <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>250</v>
       </c>
@@ -5025,8 +5072,10 @@
       <c r="C29" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F29" s="3"/>
+      <c r="H29" s="3"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>243</v>
       </c>
@@ -5036,8 +5085,10 @@
       <c r="C30" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F30" s="3"/>
+      <c r="H30" s="3"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>252</v>
       </c>
@@ -5047,8 +5098,10 @@
       <c r="C31" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F31" s="3"/>
+      <c r="H31" s="3"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>247</v>
       </c>
@@ -5058,8 +5111,10 @@
       <c r="C32" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F32" s="3"/>
+      <c r="H32" s="3"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>253</v>
       </c>
@@ -5069,8 +5124,10 @@
       <c r="C33" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F33" s="3"/>
+      <c r="H33" s="3"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>254</v>
       </c>
@@ -5080,8 +5137,10 @@
       <c r="C34" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F34" s="3"/>
+      <c r="H34" s="3"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>255</v>
       </c>
@@ -5091,8 +5150,10 @@
       <c r="C35" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F35" s="3"/>
+      <c r="H35" s="3"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>256</v>
       </c>
@@ -5102,8 +5163,10 @@
       <c r="C36" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F36" s="3"/>
+      <c r="H36" s="3"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>257</v>
       </c>
@@ -5113,8 +5176,10 @@
       <c r="C37" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F37" s="3"/>
+      <c r="H37" s="3"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>259</v>
       </c>
@@ -5124,8 +5189,10 @@
       <c r="C38" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F38" s="3"/>
+      <c r="H38" s="3"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>260</v>
       </c>
@@ -5135,8 +5202,10 @@
       <c r="C39" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F39" s="3"/>
+      <c r="H39" s="3"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>261</v>
       </c>
@@ -5146,8 +5215,10 @@
       <c r="C40" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F40" s="3"/>
+      <c r="H40" s="3"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>262</v>
       </c>
@@ -5157,8 +5228,10 @@
       <c r="C41" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F41" s="3"/>
+      <c r="H41" s="3"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>263</v>
       </c>
@@ -5168,8 +5241,10 @@
       <c r="C42" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F42" s="3"/>
+      <c r="H42" s="3"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>264</v>
       </c>
@@ -5179,8 +5254,10 @@
       <c r="C43" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F43" s="3"/>
+      <c r="H43" s="3"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>265</v>
       </c>
@@ -5190,8 +5267,10 @@
       <c r="C44" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F44" s="3"/>
+      <c r="H44" s="3"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>266</v>
       </c>
@@ -5201,8 +5280,10 @@
       <c r="C45" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F45" s="3"/>
+      <c r="H45" s="3"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>267</v>
       </c>
@@ -5212,8 +5293,10 @@
       <c r="C46" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F46" s="3"/>
+      <c r="H46" s="3"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>268</v>
       </c>
@@ -5223,8 +5306,10 @@
       <c r="C47" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F47" s="3"/>
+      <c r="H47" s="3"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>269</v>
       </c>
@@ -5234,8 +5319,10 @@
       <c r="C48" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F48" s="3"/>
+      <c r="H48" s="3"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>270</v>
       </c>
@@ -5245,8 +5332,10 @@
       <c r="C49" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F49" s="3"/>
+      <c r="H49" s="3"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>271</v>
       </c>
@@ -5256,8 +5345,10 @@
       <c r="C50" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F50" s="3"/>
+      <c r="H50" s="3"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>272</v>
       </c>
@@ -5267,8 +5358,10 @@
       <c r="C51" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F51" s="3"/>
+      <c r="H51" s="3"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>273</v>
       </c>
@@ -5278,8 +5371,10 @@
       <c r="C52" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F52" s="3"/>
+      <c r="H52" s="3"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>274</v>
       </c>
@@ -5289,8 +5384,10 @@
       <c r="C53" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F53" s="3"/>
+      <c r="H53" s="3"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>245</v>
       </c>
@@ -5300,8 +5397,10 @@
       <c r="C54" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F54" s="3"/>
+      <c r="H54" s="3"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>275</v>
       </c>
@@ -5311,8 +5410,10 @@
       <c r="C55" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F55" s="3"/>
+      <c r="H55" s="3"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>276</v>
       </c>
@@ -5322,8 +5423,10 @@
       <c r="C56" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F56" s="3"/>
+      <c r="H56" s="3"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>277</v>
       </c>
@@ -5333,8 +5436,10 @@
       <c r="C57" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F57" s="3"/>
+      <c r="H57" s="3"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>278</v>
       </c>
@@ -5344,8 +5449,10 @@
       <c r="C58" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F58" s="3"/>
+      <c r="H58" s="3"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>279</v>
       </c>
@@ -5355,8 +5462,10 @@
       <c r="C59" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F59" s="3"/>
+      <c r="H59" s="3"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>280</v>
       </c>
@@ -5366,8 +5475,10 @@
       <c r="C60" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F60" s="3"/>
+      <c r="H60" s="3"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>281</v>
       </c>
@@ -5377,8 +5488,10 @@
       <c r="C61" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F61" s="3"/>
+      <c r="H61" s="3"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>282</v>
       </c>
@@ -5388,8 +5501,10 @@
       <c r="C62" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F62" s="3"/>
+      <c r="H62" s="3"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>283</v>
       </c>
@@ -5399,8 +5514,10 @@
       <c r="C63" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F63" s="3"/>
+      <c r="H63" s="3"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>284</v>
       </c>
@@ -5410,8 +5527,10 @@
       <c r="C64" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F64" s="3"/>
+      <c r="H64" s="3"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>285</v>
       </c>
@@ -5421,8 +5540,10 @@
       <c r="C65" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F65" s="3"/>
+      <c r="H65" s="3"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>242</v>
       </c>
@@ -5432,8 +5553,10 @@
       <c r="C66" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F66" s="3"/>
+      <c r="H66" s="3"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>253</v>
       </c>
@@ -5443,8 +5566,10 @@
       <c r="C67" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F67" s="3"/>
+      <c r="H67" s="3"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>252</v>
       </c>
@@ -5454,8 +5579,10 @@
       <c r="C68" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F68" s="3"/>
+      <c r="H68" s="3"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>247</v>
       </c>
@@ -5465,8 +5592,10 @@
       <c r="C69" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F69" s="3"/>
+      <c r="H69" s="3"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>286</v>
       </c>
@@ -5476,8 +5605,10 @@
       <c r="C70" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F70" s="3"/>
+      <c r="H70" s="3"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>287</v>
       </c>
@@ -5487,8 +5618,10 @@
       <c r="C71" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F71" s="3"/>
+      <c r="H71" s="3"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>288</v>
       </c>
@@ -5498,8 +5631,10 @@
       <c r="C72" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F72" s="3"/>
+      <c r="H72" s="3"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>289</v>
       </c>
@@ -5509,8 +5644,10 @@
       <c r="C73" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F73" s="3"/>
+      <c r="H73" s="3"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>290</v>
       </c>
@@ -5520,8 +5657,10 @@
       <c r="C74" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F74" s="3"/>
+      <c r="H74" s="3"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>291</v>
       </c>
@@ -5531,8 +5670,10 @@
       <c r="C75" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F75" s="3"/>
+      <c r="H75" s="3"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>292</v>
       </c>
@@ -5542,8 +5683,10 @@
       <c r="C76" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F76" s="3"/>
+      <c r="H76" s="3"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>293</v>
       </c>
@@ -5553,8 +5696,10 @@
       <c r="C77" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F77" s="3"/>
+      <c r="H77" s="3"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>242</v>
       </c>
@@ -5564,8 +5709,10 @@
       <c r="C78" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F78" s="3"/>
+      <c r="H78" s="3"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>295</v>
       </c>
@@ -5575,8 +5722,10 @@
       <c r="C79" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F79" s="3"/>
+      <c r="H79" s="3"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>296</v>
       </c>
@@ -5586,8 +5735,10 @@
       <c r="C80" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F80" s="3"/>
+      <c r="H80" s="3"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>297</v>
       </c>
@@ -5597,8 +5748,10 @@
       <c r="C81" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F81" s="3"/>
+      <c r="H81" s="3"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>298</v>
       </c>
@@ -5608,8 +5761,10 @@
       <c r="C82" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F82" s="3"/>
+      <c r="H82" s="3"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>299</v>
       </c>
@@ -5619,8 +5774,10 @@
       <c r="C83" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F83" s="3"/>
+      <c r="H83" s="3"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>300</v>
       </c>
@@ -5630,8 +5787,10 @@
       <c r="C84" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F84" s="3"/>
+      <c r="H84" s="3"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>301</v>
       </c>
@@ -5641,8 +5800,10 @@
       <c r="C85" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F85" s="3"/>
+      <c r="H85" s="3"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>302</v>
       </c>
@@ -5652,8 +5813,10 @@
       <c r="C86" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F86" s="3"/>
+      <c r="H86" s="3"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>304</v>
       </c>
@@ -5663,8 +5826,10 @@
       <c r="C87" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F87" s="3"/>
+      <c r="H87" s="3"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>305</v>
       </c>
@@ -5674,8 +5839,10 @@
       <c r="C88" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F88" s="3"/>
+      <c r="H88" s="3"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>306</v>
       </c>
@@ -5685,8 +5852,10 @@
       <c r="C89" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F89" s="3"/>
+      <c r="H89" s="3"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>307</v>
       </c>
@@ -5696,8 +5865,10 @@
       <c r="C90" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F90" s="3"/>
+      <c r="H90" s="3"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>308</v>
       </c>
@@ -5707,8 +5878,10 @@
       <c r="C91" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F91" s="3"/>
+      <c r="H91" s="3"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>309</v>
       </c>
@@ -5718,8 +5891,10 @@
       <c r="C92" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F92" s="3"/>
+      <c r="H92" s="3"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>310</v>
       </c>
@@ -5729,8 +5904,10 @@
       <c r="C93" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F93" s="3"/>
+      <c r="H93" s="3"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>311</v>
       </c>
@@ -5740,8 +5917,10 @@
       <c r="C94" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F94" s="3"/>
+      <c r="H94" s="3"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>312</v>
       </c>
@@ -5751,8 +5930,10 @@
       <c r="C95" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F95" s="3"/>
+      <c r="H95" s="3"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>313</v>
       </c>
@@ -5762,8 +5943,10 @@
       <c r="C96" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F96" s="3"/>
+      <c r="H96" s="3"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>239</v>
       </c>
@@ -5773,8 +5956,10 @@
       <c r="C97" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F97" s="3"/>
+      <c r="H97" s="3"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>314</v>
       </c>
@@ -5784,8 +5969,10 @@
       <c r="C98" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F98" s="3"/>
+      <c r="H98" s="3"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>315</v>
       </c>
@@ -5795,8 +5982,10 @@
       <c r="C99" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F99" s="3"/>
+      <c r="H99" s="3"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>316</v>
       </c>
@@ -5806,8 +5995,10 @@
       <c r="C100" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F100" s="3"/>
+      <c r="H100" s="3"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>317</v>
       </c>
@@ -5817,8 +6008,10 @@
       <c r="C101" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F101" s="3"/>
+      <c r="H101" s="3"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>318</v>
       </c>
@@ -5828,8 +6021,10 @@
       <c r="C102" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F102" s="3"/>
+      <c r="H102" s="3"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>319</v>
       </c>
@@ -5839,8 +6034,10 @@
       <c r="C103" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F103" s="3"/>
+      <c r="H103" s="3"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>320</v>
       </c>
@@ -5850,8 +6047,10 @@
       <c r="C104" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F104" s="3"/>
+      <c r="H104" s="3"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>321</v>
       </c>
@@ -5861,8 +6060,10 @@
       <c r="C105" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F105" s="3"/>
+      <c r="H105" s="3"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>322</v>
       </c>
@@ -5872,8 +6073,10 @@
       <c r="C106" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F106" s="3"/>
+      <c r="H106" s="3"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>323</v>
       </c>
@@ -5883,8 +6086,10 @@
       <c r="C107" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F107" s="3"/>
+      <c r="H107" s="3"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>324</v>
       </c>
@@ -5894,8 +6099,10 @@
       <c r="C108" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F108" s="3"/>
+      <c r="H108" s="3"/>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>325</v>
       </c>
@@ -5905,8 +6112,10 @@
       <c r="C109" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F109" s="3"/>
+      <c r="H109" s="3"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>326</v>
       </c>
@@ -5916,8 +6125,10 @@
       <c r="C110" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F110" s="3"/>
+      <c r="H110" s="3"/>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>327</v>
       </c>
@@ -5927,8 +6138,10 @@
       <c r="C111" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F111" s="3"/>
+      <c r="H111" s="3"/>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>328</v>
       </c>
@@ -5938,8 +6151,10 @@
       <c r="C112" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F112" s="3"/>
+      <c r="H112" s="3"/>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>329</v>
       </c>
@@ -5949,8 +6164,10 @@
       <c r="C113" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F113" s="3"/>
+      <c r="H113" s="3"/>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>330</v>
       </c>
@@ -5960,8 +6177,10 @@
       <c r="C114" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F114" s="3"/>
+      <c r="H114" s="3"/>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>331</v>
       </c>
@@ -5971,8 +6190,10 @@
       <c r="C115" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F115" s="3"/>
+      <c r="H115" s="3"/>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>332</v>
       </c>
@@ -5982,8 +6203,10 @@
       <c r="C116" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F116" s="3"/>
+      <c r="H116" s="3"/>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>333</v>
       </c>
@@ -5993,8 +6216,10 @@
       <c r="C117" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F117" s="3"/>
+      <c r="H117" s="3"/>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>254</v>
       </c>
@@ -6004,8 +6229,10 @@
       <c r="C118" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F118" s="3"/>
+      <c r="H118" s="3"/>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>255</v>
       </c>
@@ -6015,8 +6242,10 @@
       <c r="C119" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F119" s="3"/>
+      <c r="H119" s="3"/>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>334</v>
       </c>
@@ -6026,8 +6255,10 @@
       <c r="C120" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F120" s="3"/>
+      <c r="H120" s="3"/>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>335</v>
       </c>
@@ -6037,8 +6268,10 @@
       <c r="C121" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F121" s="3"/>
+      <c r="H121" s="3"/>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>336</v>
       </c>
@@ -6048,8 +6281,10 @@
       <c r="C122" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F122" s="3"/>
+      <c r="H122" s="3"/>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>247</v>
       </c>
@@ -6059,8 +6294,10 @@
       <c r="C123" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F123" s="3"/>
+      <c r="H123" s="3"/>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>252</v>
       </c>
@@ -6070,8 +6307,10 @@
       <c r="C124" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F124" s="3"/>
+      <c r="H124" s="3"/>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>337</v>
       </c>
@@ -6081,8 +6320,10 @@
       <c r="C125" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F125" s="3"/>
+      <c r="H125" s="3"/>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>338</v>
       </c>
@@ -6092,8 +6333,10 @@
       <c r="C126" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F126" s="3"/>
+      <c r="H126" s="3"/>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>339</v>
       </c>
@@ -6103,8 +6346,10 @@
       <c r="C127" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F127" s="3"/>
+      <c r="H127" s="3"/>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>340</v>
       </c>
@@ -6114,8 +6359,10 @@
       <c r="C128" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F128" s="3"/>
+      <c r="H128" s="3"/>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>341</v>
       </c>
@@ -6125,8 +6372,10 @@
       <c r="C129" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F129" s="3"/>
+      <c r="H129" s="3"/>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>342</v>
       </c>
@@ -6136,8 +6385,10 @@
       <c r="C130" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F130" s="3"/>
+      <c r="H130" s="3"/>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>343</v>
       </c>
@@ -6147,8 +6398,10 @@
       <c r="C131" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F131" s="3"/>
+      <c r="H131" s="3"/>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>344</v>
       </c>
@@ -6158,8 +6411,10 @@
       <c r="C132" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F132" s="3"/>
+      <c r="H132" s="3"/>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>345</v>
       </c>
@@ -6169,8 +6424,10 @@
       <c r="C133" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F133" s="3"/>
+      <c r="H133" s="3"/>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>346</v>
       </c>
@@ -6180,8 +6437,10 @@
       <c r="C134" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F134" s="3"/>
+      <c r="H134" s="3"/>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>347</v>
       </c>
@@ -6191,8 +6450,10 @@
       <c r="C135" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F135" s="3"/>
+      <c r="H135" s="3"/>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>348</v>
       </c>
@@ -6202,8 +6463,10 @@
       <c r="C136" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F136" s="3"/>
+      <c r="H136" s="3"/>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>349</v>
       </c>
@@ -6213,8 +6476,10 @@
       <c r="C137" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F137" s="3"/>
+      <c r="H137" s="3"/>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>350</v>
       </c>
@@ -6224,8 +6489,10 @@
       <c r="C138" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F138" s="3"/>
+      <c r="H138" s="3"/>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>351</v>
       </c>
@@ -6235,8 +6502,10 @@
       <c r="C139" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F139" s="3"/>
+      <c r="H139" s="3"/>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>352</v>
       </c>
@@ -6246,8 +6515,10 @@
       <c r="C140" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F140" s="3"/>
+      <c r="H140" s="3"/>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>353</v>
       </c>
@@ -6257,8 +6528,10 @@
       <c r="C141" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F141" s="3"/>
+      <c r="H141" s="3"/>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>354</v>
       </c>
@@ -6268,8 +6541,10 @@
       <c r="C142" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F142" s="3"/>
+      <c r="H142" s="3"/>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>355</v>
       </c>
@@ -6279,8 +6554,10 @@
       <c r="C143" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F143" s="3"/>
+      <c r="H143" s="3"/>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>356</v>
       </c>
@@ -6290,8 +6567,10 @@
       <c r="C144" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F144" s="3"/>
+      <c r="H144" s="3"/>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>239</v>
       </c>
@@ -6301,8 +6580,10 @@
       <c r="C145" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F145" s="3"/>
+      <c r="H145" s="3"/>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>357</v>
       </c>
@@ -6312,8 +6593,10 @@
       <c r="C146" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F146" s="3"/>
+      <c r="H146" s="3"/>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>359</v>
       </c>
@@ -6323,8 +6606,10 @@
       <c r="C147" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F147" s="3"/>
+      <c r="H147" s="3"/>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>360</v>
       </c>
@@ -6334,8 +6619,10 @@
       <c r="C148" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F148" s="3"/>
+      <c r="H148" s="3"/>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>361</v>
       </c>
@@ -6345,8 +6632,10 @@
       <c r="C149" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F149" s="3"/>
+      <c r="H149" s="3"/>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>245</v>
       </c>
@@ -6357,7 +6646,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>362</v>
       </c>
@@ -6368,7 +6657,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>363</v>
       </c>
@@ -6379,7 +6668,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>364</v>
       </c>
@@ -6390,7 +6679,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>283</v>
       </c>
@@ -6401,7 +6690,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>275</v>
       </c>
@@ -6412,7 +6701,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>365</v>
       </c>
@@ -6423,7 +6712,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>366</v>
       </c>
@@ -6434,7 +6723,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>271</v>
       </c>
@@ -6445,7 +6734,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>277</v>
       </c>
@@ -6456,7 +6745,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>284</v>
       </c>

</xml_diff>